<commit_message>
added banking details page
</commit_message>
<xml_diff>
--- a/TestData/SR_Functional.xlsx
+++ b/TestData/SR_Functional.xlsx
@@ -4,21 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" activeTab="4"/>
+    <workbookView windowWidth="18530" windowHeight="7070" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Email" sheetId="1" r:id="rId1"/>
     <sheet name="Mobilenumber" sheetId="2" r:id="rId2"/>
     <sheet name="password" sheetId="3" r:id="rId3"/>
     <sheet name="Confirmpassword" sheetId="4" r:id="rId4"/>
-    <sheet name="PDPopuperror" sheetId="5" r:id="rId5"/>
+    <sheet name="PersonalDetailPopupError" sheetId="5" r:id="rId5"/>
+    <sheet name="CompanyName" sheetId="6" r:id="rId6"/>
+    <sheet name="CompanyEmail" sheetId="7" r:id="rId7"/>
+    <sheet name="CompanyAddress" sheetId="8" r:id="rId8"/>
+    <sheet name="CompanyPhoneNo" sheetId="9" r:id="rId9"/>
+    <sheet name="Pincode" sheetId="10" r:id="rId10"/>
+    <sheet name="CompanyDetailPopupError" sheetId="11" r:id="rId11"/>
+    <sheet name="AccountNumber" sheetId="12" r:id="rId12"/>
+    <sheet name="ConfirmAccountNumber" sheetId="13" r:id="rId13"/>
+    <sheet name="IFSCCode" sheetId="14" r:id="rId14"/>
+    <sheet name="BankingDetailPopupError" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>Email</t>
   </si>
@@ -104,22 +114,160 @@
     <t>mrinalini</t>
   </si>
   <si>
+    <t>alert@enercent.co</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>suraj</t>
+  </si>
+  <si>
+    <t>sjdhsbc@gmail.com</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>sA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s </t>
+  </si>
+  <si>
+    <t>@1</t>
+  </si>
+  <si>
+    <t>CompanyEmail</t>
+  </si>
+  <si>
+    <t>!!!@#$@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CompanyAddress</t>
+  </si>
+  <si>
+    <t>Ac</t>
+  </si>
+  <si>
+    <t>/'</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>a,</t>
+  </si>
+  <si>
+    <t>,1</t>
+  </si>
+  <si>
+    <t>@@</t>
+  </si>
+  <si>
+    <t>Company Mobile Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>asd12</t>
+  </si>
+  <si>
+    <t>@/,</t>
+  </si>
+  <si>
+    <t>Company Phone Number</t>
+  </si>
+  <si>
+    <t>Company Email Address</t>
+  </si>
+  <si>
+    <t>Company Address</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>jshdjd@gmail.com</t>
+  </si>
+  <si>
+    <t>dsdjdsds</t>
+  </si>
+  <si>
+    <t>MAHARAS</t>
+  </si>
+  <si>
+    <t>NANDED</t>
+  </si>
+  <si>
+    <t>nskdajdak</t>
+  </si>
+  <si>
     <t>suraj.k@antino.io</t>
   </si>
   <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>suraj</t>
-  </si>
-  <si>
-    <t>sbkd@gmail.com</t>
-  </si>
-  <si>
-    <t>rahul</t>
-  </si>
-  <si>
-    <t>shdjs@gmail.com</t>
+    <t>surajsdskd</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>ashgs</t>
+  </si>
+  <si>
+    <t>@!?</t>
+  </si>
+  <si>
+    <t>Confirm Account Number</t>
+  </si>
+  <si>
+    <t>@!/</t>
+  </si>
+  <si>
+    <t>kshs</t>
+  </si>
+  <si>
+    <t>IFSC Code</t>
+  </si>
+  <si>
+    <t>@!/_,</t>
+  </si>
+  <si>
+    <t>12349AHAH1J</t>
+  </si>
+  <si>
+    <t>ASB10AHSN12</t>
+  </si>
+  <si>
+    <t>1234AHA12JA</t>
+  </si>
+  <si>
+    <t>Account Holder Name</t>
+  </si>
+  <si>
+    <t>Select Bank</t>
+  </si>
+  <si>
+    <t>Automation Testing</t>
+  </si>
+  <si>
+    <t>icici</t>
+  </si>
+  <si>
+    <t>ICIC0000280</t>
+  </si>
+  <si>
+    <t>SBIN0125620</t>
   </si>
 </sst>
 </file>
@@ -127,13 +275,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -171,16 +327,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,14 +340,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -225,14 +366,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -244,6 +377,29 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,7 +421,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,13 +440,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -300,181 +456,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,36 +655,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,6 +718,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -600,164 +741,176 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -766,7 +919,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1091,7 +1259,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7"/>
@@ -1100,40 +1268,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1141,6 +1309,517 @@
   <hyperlinks>
     <hyperlink ref="A8" r:id="rId1" display=".@gmail.com"/>
   </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
+  <cols>
+    <col min="1" max="1" width="9.90909090909091" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="14.9090909090909" customWidth="1"/>
+    <col min="2" max="2" width="22.0909090909091" customWidth="1"/>
+    <col min="3" max="3" width="21.1818181818182" customWidth="1"/>
+    <col min="4" max="4" width="19.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="11.9090909090909" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3">
+        <v>9834452503</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="3">
+        <v>431603</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="3">
+        <v>9834452509</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="3">
+        <v>431603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9834452503</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="3">
+        <v>431603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9834452503</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="3">
+        <v>121227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9834452509</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3">
+        <v>431603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="3">
+        <v>9834452509</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="3">
+        <v>431603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3">
+        <v>9834452509</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="3">
+        <v>121227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3">
+        <v>9834452503</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3">
+        <v>121227</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="jshdjd@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="jshdjd@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="suraj.k@antino.io" tooltip="mailto:suraj.k@antino.io"/>
+    <hyperlink ref="C5" r:id="rId1" display="jshdjd@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId1" display="jshdjd@gmail.com"/>
+    <hyperlink ref="C7" r:id="rId2" display="suraj.k@antino.io" tooltip="mailto:suraj.k@antino.io"/>
+    <hyperlink ref="C8" r:id="rId2" display="suraj.k@antino.io" tooltip="mailto:suraj.k@antino.io"/>
+    <hyperlink ref="C9" r:id="rId2" display="suraj.k@antino.io" tooltip="mailto:suraj.k@antino.io"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
+  <cols>
+    <col min="1" max="1" width="16.1818181818182" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
+  <cols>
+    <col min="1" max="1" width="22.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="12.5454545454545" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3">
+        <v>54321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="19.9090909090909" customWidth="1"/>
+    <col min="2" max="2" width="17.8181818181818" customWidth="1"/>
+    <col min="3" max="3" width="22.3636363636364" customWidth="1"/>
+    <col min="4" max="4" width="17.2727272727273" customWidth="1"/>
+    <col min="5" max="5" width="14.6363636363636" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2">
+        <v>82387287</v>
+      </c>
+      <c r="C3" s="2">
+        <v>82387287</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="C4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1152,7 +1831,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A1" sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6"/>
@@ -1162,35 +1841,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>12345678</v>
       </c>
     </row>
@@ -1215,30 +1894,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1263,30 +1942,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1299,13 +1978,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
     <col min="2" max="2" width="21.0909090909091" customWidth="1"/>
@@ -1339,19 +2018,19 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C2">
         <v>123456</v>
       </c>
       <c r="D2">
-        <v>9836720278</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>9834452509</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1359,55 +2038,256 @@
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C3">
         <v>123456</v>
       </c>
       <c r="D3">
-        <v>9836720278</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>1212121212</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4">
-        <v>123456</v>
-      </c>
-      <c r="D4">
-        <v>9834452509</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="F3" s="9" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="suraj.k@antino.io"/>
+    <hyperlink ref="B2" r:id="rId1" display="alert@enercent.co" tooltip="mailto:alert@enercent.co"/>
     <hyperlink ref="E2" r:id="rId2" display="Test@123"/>
     <hyperlink ref="F2" r:id="rId2" display="Test@123"/>
-    <hyperlink ref="B3" r:id="rId3" display="sbkd@gmail.com"/>
     <hyperlink ref="E3" r:id="rId2" display="Test@123"/>
     <hyperlink ref="F3" r:id="rId2" display="Test@123"/>
-    <hyperlink ref="B4" r:id="rId4" display="shdjs@gmail.com"/>
-    <hyperlink ref="E4" r:id="rId2" display="Test@123"/>
-    <hyperlink ref="F4" r:id="rId2" display="Test@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="15.4545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="19.8181818181818" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" display=".@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="18.4545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>